<commit_message>
Helps if I save the changed table instead of the source table
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/2020Results.xlsx
+++ b/Tests/Validation/Wheat/2020Results.xlsx
@@ -443,12 +443,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Wheat.Leaf.AppearedCohortNo</t>
+          <t>Wheat.Leaf.Tips</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Wheat.Leaf.ExpandedCohortNo</t>
+          <t>Wheat.Leaf.Ligules</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -488,7 +488,7 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Wheat.Structure.TotalStemPopn</t>
+          <t>Wheat.Leaf.StemPopulation</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">

</xml_diff>